<commit_message>
adding multivalue cells to DD's excel
</commit_message>
<xml_diff>
--- a/data_dictionary/profiles.xlsx
+++ b/data_dictionary/profiles.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="408">
   <si>
     <t>acl</t>
   </si>
@@ -282,6 +282,72 @@
     <t>http://purl.org/dc/terms/language</t>
   </si>
   <si>
+    <t>http://id.loc.gov/vocabulary/iso639-2/ita</t>
+  </si>
+  <si>
+    <t>Italian</t>
+  </si>
+  <si>
+    <t>http://id.loc.gov/vocabulary/iso639-2/rus</t>
+  </si>
+  <si>
+    <t>Russian</t>
+  </si>
+  <si>
+    <t>http://id.loc.gov/vocabulary/iso639-2/zxx</t>
+  </si>
+  <si>
+    <t>No linguistic content</t>
+  </si>
+  <si>
+    <t>http://id.loc.gov/vocabulary/iso639-2/eng</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>http://id.loc.gov/vocabulary/iso639-2/fre</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>http://id.loc.gov/vocabulary/iso639-2/por</t>
+  </si>
+  <si>
+    <t>Portuguese</t>
+  </si>
+  <si>
+    <t>http://id.loc.gov/vocabulary/iso639-2/zho</t>
+  </si>
+  <si>
+    <t>Chinese</t>
+  </si>
+  <si>
+    <t>http://id.loc.gov/vocabulary/iso639-2/vie</t>
+  </si>
+  <si>
+    <t>Vietnamese</t>
+  </si>
+  <si>
+    <t>http://purl.org/dc/terms/license</t>
+  </si>
+  <si>
+    <t>http://id.loc.gov/vocabulary/iso639-2/ipk</t>
+  </si>
+  <si>
+    <t>Inupiaq</t>
+  </si>
+  <si>
+    <t>http://id.loc.gov/vocabulary/iso639-2/spa</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
     <t>http://id.loc.gov/vocabulary/iso639-2/ukr</t>
   </si>
   <si>
@@ -306,72 +372,6 @@
     <t>Other language</t>
   </si>
   <si>
-    <t>http://id.loc.gov/vocabulary/iso639-2/ita</t>
-  </si>
-  <si>
-    <t>Italian</t>
-  </si>
-  <si>
-    <t>http://id.loc.gov/vocabulary/iso639-2/rus</t>
-  </si>
-  <si>
-    <t>Russian</t>
-  </si>
-  <si>
-    <t>http://id.loc.gov/vocabulary/iso639-2/zxx</t>
-  </si>
-  <si>
-    <t>No linguistic content</t>
-  </si>
-  <si>
-    <t>http://id.loc.gov/vocabulary/iso639-2/eng</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>http://purl.org/dc/terms/license</t>
-  </si>
-  <si>
-    <t>http://id.loc.gov/vocabulary/iso639-2/fre</t>
-  </si>
-  <si>
-    <t>French</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>http://id.loc.gov/vocabulary/iso639-2/por</t>
-  </si>
-  <si>
-    <t>Portuguese</t>
-  </si>
-  <si>
-    <t>http://id.loc.gov/vocabulary/iso639-2/zho</t>
-  </si>
-  <si>
-    <t>Chinese</t>
-  </si>
-  <si>
-    <t>http://id.loc.gov/vocabulary/iso639-2/vie</t>
-  </si>
-  <si>
-    <t>Vietnamese</t>
-  </si>
-  <si>
-    <t>http://id.loc.gov/vocabulary/iso639-2/ipk</t>
-  </si>
-  <si>
-    <t>Inupiaq</t>
-  </si>
-  <si>
-    <t>http://id.loc.gov/vocabulary/iso639-2/spa</t>
-  </si>
-  <si>
-    <t>Spanish</t>
-  </si>
-  <si>
     <t>http://creativecommons.org/licenses/by-nc-nd/4.0/</t>
   </si>
   <si>
@@ -492,7 +492,7 @@
     <t>ebu : dateIngested</t>
   </si>
   <si>
-    <t>map first to info:createdDate. if not available, map next to fedora:created</t>
+    <t>backward compatible with info : createdDate || backward compatible with fedora : created || map first to info:createdDate. if not available, map next to fedora:created</t>
   </si>
   <si>
     <t>ual : hydraNoid</t>
@@ -591,7 +591,7 @@
     <t>ual : fedora3UUID</t>
   </si>
   <si>
-    <t>http://terms.library.library.ca/identifiers/fedora3uuid</t>
+    <t>ual : id/fedora3uuid || http://terms.library.library.ca/identifiers/fedora3uuid</t>
   </si>
   <si>
     <t>rdf : type</t>
@@ -609,7 +609,7 @@
     <t>pcdm : memberOf</t>
   </si>
   <si>
-    <t>http://terms.library.library.ca/identifiers/belongsToCommunity</t>
+    <t>ual : id/belongsToCommunity || http://terms.library.library.ca/identifiers/belongsToCommunity</t>
   </si>
   <si>
     <t>indicates community inheritence</t>
@@ -684,7 +684,7 @@
     <t>ual : nnaFile</t>
   </si>
   <si>
-    <t>ualid : halpern:nnafile</t>
+    <t>ual : id/halpern:nnafile</t>
   </si>
   <si>
     <t>legacy property</t>
@@ -708,7 +708,7 @@
     <t>type of item</t>
   </si>
   <si>
-    <t>{u'onForm': u'true', u'uri': u'http://terms.library.ualberta.ca/learningObject', u'label': u'Learning Object'}</t>
+    <t>{u'onForm': u'true', u'uri': u'bibo : Article', u'label': u'Article'} || {u'onForm': u'true', u'uri': u'bibo : Book', u'label': u'Book'} || {u'onForm': u'true', u'uri': u'bibo : Chapter', u'label': u'Chapter'} || {u'onForm': u'true', u'uri': u'bibo : Image', u'label': u'Image'} || {u'onForm': u'true', u'uri': u'bibo : Report', u'label': u'Report'} || {u'onForm': u'true', u'uri': u'ual : researchMaterial', u'label': u'Research Material'} || {u'onForm': u'true', u'uri': u'vivo : ConferencePaper', u'label': u'Conference Paper'} || {u'onForm': u'true', u'uri': u'vivo : ConferencePoster', u'label': u'Conference Poster'} || {u'onForm': u'true', u'uri': u'vivo : Dataset', u'label': u'Dataset'} || {u'onForm': u'true', u'uri': u'vivo : Review', u'label': u'Review'} || {u'onForm': u'true', u'uri': u'ual : learningObject', u'label': u'Learning Object'}</t>
   </si>
   <si>
     <t>dcterms : license</t>
@@ -723,13 +723,13 @@
     <t>license information</t>
   </si>
   <si>
-    <t>{u'onForm': u'false', u'uri': u'http://creativecommons.org/licenses/by-nc-nd/3.0/', u'label': u'Attribution-NonCommercial-NoDerivs 3.0 Unported'}</t>
+    <t>{u'onForm': u'true', u'uri': u'http://creativecommons.org/licenses/by/4.0/', u'label': u'Attribution 4.0 International'} || {u'onForm': u'false', u'uri': u'http://creativecommons.org/licenses/by-nc/3.0/', u'label': u'Attribution-NonCommercial 3.0 Unported'} || {u'onForm': u'true', u'uri': u'http://creativecommons.org/licenses/by-sa/4.0/', u'label': u'Attribution-ShareAlike 4.0 International'} || {u'onForm': u'true', u'uri': u'http://creativecommons.org/licenses/by-nc/4.0/', u'label': u'Attribution-NonCommercial 4.0 International'} || {u'onForm': u'false', u'uri': u'http://creativecommons.org/licenses/by-nd/3.0/', u'label': u'Attribution-NoDerivs 3.0 Unported'} || {u'onForm': u'false', u'uri': u'http://creativecommons.org/licenses/by/3.0/', u'label': u'Attribution 3.0 Unported'} || {u'onForm': u'true', u'uri': u'http://creativecommons.org/licenses/by-nc-nd/4.0/', u'label': u'Attribution-NonCommercial-NoDerivatives 4.0 International'} || {u'onForm': u'false', u'uri': u'http://creativecommons.org/licenses/by-sa/3.0/', u'label': u'Attribution-ShareAlike 3.0 Unported'} || {u'onForm': u'true', u'uri': u'http://creativecommons.org/publicdomain/zero/1.0/', u'label': u'CC0 1.0 Universal'} || {u'onForm': u'true', u'uri': u'http://creativecommons.org/licenses/by-nd/4.0/', u'label': u'Attribution-NoDerivatives 4.0 International'} || {u'onForm': u'true', u'uri': u'http://creativecommons.org/publicdomain/mark/1.0/', u'label': u'Public Domain Mark 1.0'} || {u'onForm': u'false', u'uri': u'http://creativecommons.org/licenses/by-nc-sa/3.0/', u'label': u'Attribution-NonCommercial-ShareAlike 3.0 Unported'} || {u'onForm': u'true', u'uri': u'http://creativecommons.org/licenses/by-nc-sa/4.0/', u'label': u'Attribution-NonCommercial-ShareAlike 4.0 International'} || {u'onForm': u'false', u'uri': u'http://creativecommons.org/licenses/by-nc-nd/3.0/', u'label': u'Attribution-NonCommercial-NoDerivs 3.0 Unported'}</t>
   </si>
   <si>
     <t>ual : ark</t>
   </si>
   <si>
-    <t>ualid : arkid</t>
+    <t>ual : id/arkid</t>
   </si>
   <si>
     <t>archival resource key id</t>
@@ -747,7 +747,7 @@
     <t>fedora : digest</t>
   </si>
   <si>
-    <t>ualid : fedora3uuid</t>
+    <t>ual : id/fedora3uuid</t>
   </si>
   <si>
     <t>fedora 3 uuid</t>
@@ -774,7 +774,7 @@
     <t>ual : nnaItem</t>
   </si>
   <si>
-    <t>ualid : halpern:nnaitem</t>
+    <t>ual : id/halpern:nnaitem</t>
   </si>
   <si>
     <t>northern north america item id</t>
@@ -786,7 +786,7 @@
     <t>prism : doi</t>
   </si>
   <si>
-    <t>ualid : doi</t>
+    <t>ual : id/doi</t>
   </si>
   <si>
     <t>always doi (currently set to searchable (should this be changed?)</t>
@@ -807,7 +807,7 @@
     <t>ual : unicorn</t>
   </si>
   <si>
-    <t>ualid : unicorn</t>
+    <t>ual : id/unicorn</t>
   </si>
   <si>
     <t>unicorn</t>
@@ -840,10 +840,10 @@
     <t>https://github.com/ualbertalib/metadata/tree/master/data_dictionary/jupiter_ontology.md#bibostatus</t>
   </si>
   <si>
-    <t>{u'onForm': u'false', u'uri': u'http://purl.org/ontology/bibo/status#accepted', u'label': u'accepted'}</t>
-  </si>
-  <si>
-    <t>ualids : hasCollectionId</t>
+    <t>{u'onForm': u'false', u'uri': u'bibo : status#unpublished', u'label': u'unpublished'} || {u'onForm': u'true', u'uri': u'bibo : status#published', u'label': u'published'} || {u'onForm': u'true', u'uri': u'bibo : status#draft', u'label': u'draft'} || {u'onForm': u'true', u'uri': u'vivo : submitted', u'label': u'submitted'} || {u'onForm': u'false', u'uri': u'bibo : status#accepted', u'label': u'accepted'}</t>
+  </si>
+  <si>
+    <t>ual : identifiers/hasCollectionId</t>
   </si>
   <si>
     <t>indicates collection inheritance</t>
@@ -903,7 +903,7 @@
     <t>ual : ingestBatch</t>
   </si>
   <si>
-    <t>http://terms.library.library.ca/identifiers/ingestbatch</t>
+    <t>http://terms.library.library.ca/id/ingestbatch || http://terms.library.library.ca/identifiers/ingestbatch</t>
   </si>
   <si>
     <t>dcterms : alternative</t>
@@ -921,13 +921,13 @@
     <t>language</t>
   </si>
   <si>
-    <t>{u'onForm': u'true', u'uri': u'http://id.loc.gov/vocabulary/iso639-2/spa', u'label': u'Spanish'}</t>
+    <t>{u'onForm': u'true', u'uri': u'lang : ukr', u'label': u'Ukranian'} || {u'onForm': u'true', u'uri': u'lang : jpn', u'label': u'Japanese'} || {u'onForm': u'true', u'uri': u'lang : ger', u'label': u'German'} || {u'onForm': u'true', u'uri': u'ual : other', u'label': u'Other language'} || {u'onForm': u'true', u'uri': u'lang : ita', u'label': u'Italian'} || {u'onForm': u'true', u'uri': u'lang : rus', u'label': u'Russian'} || {u'onForm': u'true', u'uri': u'lang : zxx', u'label': u'No linguistic content'} || {u'onForm': u'true', u'uri': u'lang : eng', u'label': u'English'} || {u'onForm': u'true', u'uri': u'lang : fre', u'label': u'French'} || {u'onForm': u'false', u'uri': u'lang : por', u'label': u'Portuguese'} || {u'onForm': u'true', u'uri': u'lang : zho', u'label': u'Chinese'} || {u'onForm': u'false', u'uri': u'lang : vie', u'label': u'Vietnamese'} || {u'onForm': u'false', u'uri': u'lang : ipk', u'label': u'Inupiaq'} || {u'onForm': u'true', u'uri': u'lang : spa', u'label': u'Spanish'}</t>
   </si>
   <si>
     <t>ual : fedora3Handle</t>
   </si>
   <si>
-    <t>ualid : fedora3handle</t>
+    <t>ual : id/fedora3handle</t>
   </si>
   <si>
     <t>fedora 3 handle</t>
@@ -957,7 +957,7 @@
     <t>ual : commiteeMember</t>
   </si>
   <si>
-    <t>ualrole : thesiscommitteemember</t>
+    <t>ual : role/thesiscommitteemember</t>
   </si>
   <si>
     <t>commitee member</t>
@@ -972,7 +972,7 @@
     <t>ual : graduationDate</t>
   </si>
   <si>
-    <t>ualdate : graduationdate</t>
+    <t>ual : date/graduationdate</t>
   </si>
   <si>
     <t>graduation date</t>
@@ -1005,7 +1005,7 @@
     <t>ual : proquest</t>
   </si>
   <si>
-    <t>ualid : proquest</t>
+    <t>ual : id/proquest</t>
   </si>
   <si>
     <t>proquest</t>
@@ -1017,7 +1017,7 @@
     <t>ual : specialization</t>
   </si>
   <si>
-    <t>ualthesis : specialization</t>
+    <t>ual : thesis/specialization</t>
   </si>
   <si>
     <t>specialization</t>
@@ -1056,7 +1056,7 @@
     <t>{u'onForm': u'False', u'uri': u'bibo : Thesis', u'label': u'Thesis'}</t>
   </si>
   <si>
-    <t>thesis always belong to collection 44558t416</t>
+    <t>indicates collection inheritance || thesis always belong to collection 44558t416</t>
   </si>
   <si>
     <t>swrc : institution</t>
@@ -1074,7 +1074,7 @@
     <t>degree grantor</t>
   </si>
   <si>
-    <t>{u'onForm': u'true', u'uri': u'lcn : n2009054054', u'label': u"St. Stephen's College"}</t>
+    <t>{u'onForm': u'true', u'uri': u'lcn : n79058482', u'label': u'University of Alberta'} || {u'onForm': u'true', u'uri': u'lcn : n2009054054', u'label': u"St. Stephen's College"}</t>
   </si>
   <si>
     <t>ual : dissertant</t>
@@ -1116,13 +1116,16 @@
     <t>https://github.com/ualbertalib/metadata/tree/master/data_dictionary/jupiter_ontology.md#bibodegree</t>
   </si>
   <si>
+    <t>{u'onForm': u'true', u'uri': u'lang : ita', u'label': u'Italian'} || {u'onForm': u'true', u'uri': u'lang : rus', u'label': u'Russian'} || {u'onForm': u'true', u'uri': u'lang : zxx', u'label': u'No linguistic content'} || {u'onForm': u'true', u'uri': u'lang : eng', u'label': u'English'} || {u'onForm': u'true', u'uri': u'lang : fre', u'label': u'French'} || {u'onForm': u'false', u'uri': u'lang : por', u'label': u'Portuguese'} || {u'onForm': u'true', u'uri': u'lang : zho', u'label': u'Chinese'} || {u'onForm': u'false', u'uri': u'lang : vie', u'label': u'Vietnamese'} || {u'onForm': u'false', u'uri': u'lang : ipk', u'label': u'Inupiaq'} || {u'onForm': u'true', u'uri': u'lang : spa', u'label': u'Spanish'} || {u'onForm': u'true', u'uri': u'lang : ukr', u'label': u'Ukranian'} || {u'onForm': u'true', u'uri': u'lang : jpn', u'label': u'Japanese'} || {u'onForm': u'true', u'uri': u'lang : ger', u'label': u'German'} || {u'onForm': u'true', u'uri': u'ual : other', u'label': u'Other language'}</t>
+  </si>
+  <si>
     <t>https://github.com/ualbertalib/metadata/tree/master/data_dictionary/jupiter_ontology.md#ualfedora3handle</t>
   </si>
   <si>
     <t>ual : thesisLevel</t>
   </si>
   <si>
-    <t>ualthesis : thesislevel</t>
+    <t>ual : thesis/thesislevel</t>
   </si>
   <si>
     <t>thesis level</t>
@@ -1197,10 +1200,13 @@
     <t>etd_ms : rights</t>
   </si>
   <si>
+    <t>role='committeemember' || etd_ms : contributor</t>
+  </si>
+  <si>
     <t>etd_ms : contributor</t>
   </si>
   <si>
-    <t>etd_ms : level</t>
+    <t>etd_ms : degree || etd_ms : level</t>
   </si>
   <si>
     <t>etd_ms : date</t>
@@ -1212,7 +1218,7 @@
     <t>etd_ms : title</t>
   </si>
   <si>
-    <t>etd_ms : discipline</t>
+    <t>etd_ms : degree || etd_ms : discipline</t>
   </si>
   <si>
     <t>etd_ms : description</t>
@@ -1221,6 +1227,9 @@
     <t>etd_ms : identifier</t>
   </si>
   <si>
+    <t>role='advisor' || etd_ms : contributor</t>
+  </si>
+  <si>
     <t>etd_ms : subject</t>
   </si>
   <si>
@@ -1230,7 +1239,7 @@
     <t>etd_ms : creator</t>
   </si>
   <si>
-    <t>etd_ms : name</t>
+    <t>etd_ms : degree || etd_ms : name</t>
   </si>
   <si>
     <t>etd_ms : alternativeTitle</t>
@@ -2000,13 +2009,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="B10" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="C10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2014,40 +2023,40 @@
         <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="B12" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="C12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="C13" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D13" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="B14" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="C14" t="s">
         <v>106</v>
@@ -2069,7 +2078,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="B16" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="C16" t="s">
         <v>110</v>
@@ -2080,7 +2089,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="B17" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="C17" t="s">
         <v>112</v>
@@ -2113,7 +2122,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="B20" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C20" t="s">
         <v>118</v>
@@ -2157,7 +2166,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="B24" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C24" t="s">
         <v>126</v>
@@ -2179,7 +2188,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="B26" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C26" t="s">
         <v>130</v>
@@ -2193,7 +2202,7 @@
         <v>132</v>
       </c>
       <c r="B27" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C27" t="s">
         <v>133</v>
@@ -2237,7 +2246,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="B31" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C31" t="s">
         <v>141</v>
@@ -2254,10 +2263,10 @@
         <v>80</v>
       </c>
       <c r="C32" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="D32" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -2265,10 +2274,10 @@
         <v>80</v>
       </c>
       <c r="C33" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="D33" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -2276,10 +2285,10 @@
         <v>80</v>
       </c>
       <c r="C34" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="D34" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -2287,10 +2296,10 @@
         <v>80</v>
       </c>
       <c r="C35" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="D35" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -2298,10 +2307,10 @@
         <v>80</v>
       </c>
       <c r="C36" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D36" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -2309,10 +2318,10 @@
         <v>80</v>
       </c>
       <c r="C37" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D37" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -2320,10 +2329,10 @@
         <v>80</v>
       </c>
       <c r="C38" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D38" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -2331,10 +2340,10 @@
         <v>80</v>
       </c>
       <c r="C39" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D39" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -2342,21 +2351,21 @@
         <v>80</v>
       </c>
       <c r="C40" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="D40" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="B41" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C41" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D41" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -2364,32 +2373,32 @@
         <v>80</v>
       </c>
       <c r="C42" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D42" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="B43" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C43" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D43" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="B44" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" t="s">
+        <v>104</v>
+      </c>
+      <c r="D44" t="s">
         <v>105</v>
-      </c>
-      <c r="C44" t="s">
-        <v>112</v>
-      </c>
-      <c r="D44" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -2397,10 +2406,10 @@
         <v>80</v>
       </c>
       <c r="C45" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D45" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2502,7 +2511,7 @@
         <v>158</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -2527,19 +2536,19 @@
         <v>160</v>
       </c>
       <c r="C5" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D5" t="s">
         <v>162</v>
       </c>
       <c r="E5" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F5" t="s">
         <v>163</v>
       </c>
       <c r="G5" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="H5" t="s">
         <v>164</v>
@@ -2548,16 +2557,16 @@
         <v>165</v>
       </c>
       <c r="J5" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K5" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="L5" t="s">
         <v>166</v>
       </c>
       <c r="M5" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -2568,19 +2577,19 @@
         <v>160</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D6" t="s">
         <v>167</v>
       </c>
       <c r="E6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F6" t="s">
         <v>163</v>
       </c>
       <c r="G6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="H6" t="s">
         <v>168</v>
@@ -2598,10 +2607,10 @@
         <v>169</v>
       </c>
       <c r="M6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="N6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="O6" t="s">
         <v>168</v>
@@ -2615,13 +2624,13 @@
         <v>171</v>
       </c>
       <c r="C7" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D7" t="s">
         <v>170</v>
       </c>
       <c r="E7" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F7" t="s">
         <v>163</v>
@@ -2850,19 +2859,19 @@
         <v>179</v>
       </c>
       <c r="C12" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D12" t="s">
         <v>180</v>
       </c>
       <c r="E12" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F12" t="s">
         <v>163</v>
       </c>
       <c r="G12" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="H12" t="s">
         <v>181</v>
@@ -2871,16 +2880,16 @@
         <v>182</v>
       </c>
       <c r="J12" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K12" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="L12" t="s">
         <v>183</v>
       </c>
       <c r="M12" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="N12" t="s">
         <v>160</v>
@@ -3392,13 +3401,13 @@
         <v>162</v>
       </c>
       <c r="D5" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E5" t="s">
         <v>163</v>
       </c>
       <c r="F5" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="G5" t="s">
         <v>164</v>
@@ -3407,19 +3416,19 @@
         <v>165</v>
       </c>
       <c r="I5" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J5" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K5" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="L5" t="s">
         <v>166</v>
       </c>
       <c r="M5" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -3433,13 +3442,13 @@
         <v>167</v>
       </c>
       <c r="D6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E6" t="s">
         <v>163</v>
       </c>
       <c r="F6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="G6" t="s">
         <v>168</v>
@@ -3451,7 +3460,7 @@
         <v>80</v>
       </c>
       <c r="J6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K6" t="s">
         <v>80</v>
@@ -3460,10 +3469,10 @@
         <v>169</v>
       </c>
       <c r="M6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="N6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="O6" t="s">
         <v>168</v>
@@ -3480,7 +3489,7 @@
         <v>170</v>
       </c>
       <c r="D7" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E7" t="s">
         <v>163</v>
@@ -3498,7 +3507,7 @@
         <v>80</v>
       </c>
       <c r="J7" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K7" t="s">
         <v>80</v>
@@ -3715,13 +3724,13 @@
         <v>180</v>
       </c>
       <c r="D12" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E12" t="s">
         <v>163</v>
       </c>
       <c r="F12" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="G12" t="s">
         <v>181</v>
@@ -3730,19 +3739,19 @@
         <v>182</v>
       </c>
       <c r="I12" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J12" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K12" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="L12" t="s">
         <v>183</v>
       </c>
       <c r="M12" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="N12" t="s">
         <v>160</v>
@@ -3950,13 +3959,13 @@
         <v>195</v>
       </c>
       <c r="D17" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E17" t="s">
         <v>160</v>
       </c>
       <c r="F17" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="G17" t="s">
         <v>160</v>
@@ -3968,7 +3977,7 @@
         <v>80</v>
       </c>
       <c r="J17" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K17" t="s">
         <v>80</v>
@@ -4118,7 +4127,7 @@
         <v>160</v>
       </c>
       <c r="J20" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K20" t="s">
         <v>160</v>
@@ -4339,7 +4348,7 @@
         <v>80</v>
       </c>
       <c r="F6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="G6" t="s">
         <v>202</v>
@@ -4348,13 +4357,13 @@
         <v>182</v>
       </c>
       <c r="I6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="L6" t="s">
         <v>80</v>
@@ -4371,10 +4380,10 @@
         <v>205</v>
       </c>
       <c r="D7" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E7" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F7" t="s">
         <v>160</v>
@@ -4389,13 +4398,13 @@
         <v>80</v>
       </c>
       <c r="J7" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K7" t="s">
         <v>80</v>
       </c>
       <c r="L7" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M7" t="s">
         <v>163</v>
@@ -4515,7 +4524,7 @@
         <v>80</v>
       </c>
       <c r="E10" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F10" t="s">
         <v>160</v>
@@ -4536,7 +4545,7 @@
         <v>80</v>
       </c>
       <c r="L10" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M10" t="s">
         <v>163</v>
@@ -4562,10 +4571,10 @@
         <v>215</v>
       </c>
       <c r="D11" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E11" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F11" t="s">
         <v>160</v>
@@ -4580,13 +4589,13 @@
         <v>80</v>
       </c>
       <c r="J11" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K11" t="s">
         <v>80</v>
       </c>
       <c r="L11" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M11" t="s">
         <v>163</v>
@@ -4712,10 +4721,10 @@
         <v>221</v>
       </c>
       <c r="D14" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E14" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F14" t="s">
         <v>160</v>
@@ -4727,16 +4736,16 @@
         <v>165</v>
       </c>
       <c r="I14" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J14" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K14" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="L14" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M14" t="s">
         <v>163</v>
@@ -4765,7 +4774,7 @@
         <v>80</v>
       </c>
       <c r="E15" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F15" t="s">
         <v>160</v>
@@ -4780,7 +4789,7 @@
         <v>80</v>
       </c>
       <c r="J15" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K15" t="s">
         <v>80</v>
@@ -4868,10 +4877,10 @@
         <v>205</v>
       </c>
       <c r="D17" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E17" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F17" t="s">
         <v>160</v>
@@ -4886,13 +4895,13 @@
         <v>80</v>
       </c>
       <c r="J17" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K17" t="s">
         <v>80</v>
       </c>
       <c r="L17" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M17" t="s">
         <v>163</v>
@@ -4974,7 +4983,7 @@
         <v>160</v>
       </c>
       <c r="D19" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E19" t="s">
         <v>80</v>
@@ -4992,7 +5001,7 @@
         <v>80</v>
       </c>
       <c r="J19" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K19" t="s">
         <v>80</v>
@@ -5027,10 +5036,10 @@
         <v>160</v>
       </c>
       <c r="D20" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E20" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F20" t="s">
         <v>160</v>
@@ -5042,16 +5051,16 @@
         <v>165</v>
       </c>
       <c r="I20" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J20" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K20" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="L20" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M20" t="s">
         <v>163</v>
@@ -5345,10 +5354,10 @@
         <v>221</v>
       </c>
       <c r="D26" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E26" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F26" t="s">
         <v>160</v>
@@ -5360,16 +5369,16 @@
         <v>165</v>
       </c>
       <c r="I26" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J26" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K26" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="L26" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M26" t="s">
         <v>163</v>
@@ -5416,7 +5425,7 @@
         <v>80</v>
       </c>
       <c r="J27" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K27" t="s">
         <v>80</v>
@@ -5451,10 +5460,10 @@
         <v>160</v>
       </c>
       <c r="D28" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E28" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F28" t="s">
         <v>80</v>
@@ -5469,13 +5478,13 @@
         <v>80</v>
       </c>
       <c r="J28" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K28" t="s">
         <v>80</v>
       </c>
       <c r="L28" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M28" t="s">
         <v>163</v>
@@ -5557,10 +5566,10 @@
         <v>221</v>
       </c>
       <c r="D30" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E30" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F30" t="s">
         <v>160</v>
@@ -5572,16 +5581,16 @@
         <v>165</v>
       </c>
       <c r="I30" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J30" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K30" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="L30" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M30" t="s">
         <v>163</v>
@@ -5610,13 +5619,13 @@
         <v>255</v>
       </c>
       <c r="D31" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E31" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F31" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="G31" t="s">
         <v>256</v>
@@ -5628,10 +5637,10 @@
         <v>80</v>
       </c>
       <c r="J31" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K31" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="L31" t="s">
         <v>80</v>
@@ -5663,10 +5672,10 @@
         <v>179</v>
       </c>
       <c r="D32" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E32" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F32" t="s">
         <v>160</v>
@@ -5678,16 +5687,16 @@
         <v>182</v>
       </c>
       <c r="I32" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J32" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K32" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="L32" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M32" t="s">
         <v>163</v>
@@ -5822,10 +5831,10 @@
         <v>221</v>
       </c>
       <c r="D35" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E35" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F35" t="s">
         <v>160</v>
@@ -5837,16 +5846,16 @@
         <v>165</v>
       </c>
       <c r="I35" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J35" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K35" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="L35" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M35" t="s">
         <v>163</v>
@@ -5893,7 +5902,7 @@
         <v>160</v>
       </c>
       <c r="J36" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K36" t="s">
         <v>160</v>
@@ -5928,10 +5937,10 @@
         <v>160</v>
       </c>
       <c r="D37" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E37" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F37" t="s">
         <v>160</v>
@@ -5952,7 +5961,7 @@
         <v>80</v>
       </c>
       <c r="L37" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M37" t="s">
         <v>163</v>
@@ -5981,10 +5990,10 @@
         <v>270</v>
       </c>
       <c r="D38" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E38" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F38" t="s">
         <v>160</v>
@@ -6002,10 +6011,10 @@
         <v>80</v>
       </c>
       <c r="K38" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="L38" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M38" t="s">
         <v>163</v>
@@ -6037,7 +6046,7 @@
         <v>80</v>
       </c>
       <c r="E39" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F39" t="s">
         <v>80</v>
@@ -6205,7 +6214,7 @@
         <v>80</v>
       </c>
       <c r="E42" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F42" t="s">
         <v>80</v>
@@ -6258,10 +6267,10 @@
         <v>160</v>
       </c>
       <c r="D43" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E43" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F43" t="s">
         <v>160</v>
@@ -6282,7 +6291,7 @@
         <v>80</v>
       </c>
       <c r="L43" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M43" t="s">
         <v>163</v>
@@ -6426,10 +6435,10 @@
         <v>215</v>
       </c>
       <c r="D46" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E46" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F46" t="s">
         <v>160</v>
@@ -6450,7 +6459,7 @@
         <v>80</v>
       </c>
       <c r="L46" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M46" t="s">
         <v>163</v>
@@ -6538,10 +6547,10 @@
         <v>215</v>
       </c>
       <c r="D48" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E48" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F48" t="s">
         <v>160</v>
@@ -6556,13 +6565,13 @@
         <v>80</v>
       </c>
       <c r="J48" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K48" t="s">
         <v>80</v>
       </c>
       <c r="L48" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M48" t="s">
         <v>163</v>
@@ -6759,10 +6768,10 @@
         <v>294</v>
       </c>
       <c r="D52" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E52" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F52" t="s">
         <v>80</v>
@@ -6777,13 +6786,13 @@
         <v>80</v>
       </c>
       <c r="J52" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K52" t="s">
         <v>80</v>
       </c>
       <c r="L52" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M52" t="s">
         <v>163</v>
@@ -6818,7 +6827,7 @@
         <v>80</v>
       </c>
       <c r="E53" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F53" t="s">
         <v>160</v>
@@ -6871,10 +6880,10 @@
         <v>221</v>
       </c>
       <c r="D54" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E54" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F54" t="s">
         <v>160</v>
@@ -6886,16 +6895,16 @@
         <v>165</v>
       </c>
       <c r="I54" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J54" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K54" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="L54" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M54" t="s">
         <v>163</v>
@@ -6930,7 +6939,7 @@
         <v>80</v>
       </c>
       <c r="E55" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F55" t="s">
         <v>80</v>
@@ -7167,7 +7176,7 @@
         <v>80</v>
       </c>
       <c r="F5" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="G5" t="s">
         <v>202</v>
@@ -7176,13 +7185,13 @@
         <v>182</v>
       </c>
       <c r="I5" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J5" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K5" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="L5" t="s">
         <v>80</v>
@@ -7223,7 +7232,7 @@
         <v>80</v>
       </c>
       <c r="L6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M6" t="s">
         <v>163</v>
@@ -7246,10 +7255,10 @@
         <v>160</v>
       </c>
       <c r="D7" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E7" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F7" t="s">
         <v>160</v>
@@ -7261,16 +7270,16 @@
         <v>165</v>
       </c>
       <c r="I7" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J7" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K7" t="s">
         <v>80</v>
       </c>
       <c r="L7" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M7" t="s">
         <v>163</v>
@@ -7293,7 +7302,7 @@
         <v>160</v>
       </c>
       <c r="D8" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E8" t="s">
         <v>80</v>
@@ -7311,7 +7320,7 @@
         <v>80</v>
       </c>
       <c r="J8" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K8" t="s">
         <v>80</v>
@@ -7546,7 +7555,7 @@
         <v>160</v>
       </c>
       <c r="E13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F13" t="s">
         <v>80</v>
@@ -7561,13 +7570,13 @@
         <v>80</v>
       </c>
       <c r="J13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K13" t="s">
         <v>80</v>
       </c>
       <c r="L13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M13" t="s">
         <v>163</v>
@@ -7643,7 +7652,7 @@
         <v>160</v>
       </c>
       <c r="D15" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E15" t="s">
         <v>80</v>
@@ -7661,7 +7670,7 @@
         <v>80</v>
       </c>
       <c r="J15" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K15" t="s">
         <v>80</v>
@@ -7693,10 +7702,10 @@
         <v>160</v>
       </c>
       <c r="D16" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E16" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F16" t="s">
         <v>160</v>
@@ -7717,7 +7726,7 @@
         <v>80</v>
       </c>
       <c r="L16" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M16" t="s">
         <v>163</v>
@@ -7793,10 +7802,10 @@
         <v>221</v>
       </c>
       <c r="D18" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E18" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F18" t="s">
         <v>160</v>
@@ -7808,16 +7817,16 @@
         <v>165</v>
       </c>
       <c r="I18" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J18" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K18" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="L18" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M18" t="s">
         <v>163</v>
@@ -7893,10 +7902,10 @@
         <v>160</v>
       </c>
       <c r="D20" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E20" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F20" t="s">
         <v>160</v>
@@ -7917,7 +7926,7 @@
         <v>80</v>
       </c>
       <c r="L20" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M20" t="s">
         <v>163</v>
@@ -7943,10 +7952,10 @@
         <v>160</v>
       </c>
       <c r="D21" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E21" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F21" t="s">
         <v>160</v>
@@ -7958,16 +7967,16 @@
         <v>182</v>
       </c>
       <c r="I21" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J21" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K21" t="s">
         <v>80</v>
       </c>
       <c r="L21" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M21" t="s">
         <v>163</v>
@@ -8093,10 +8102,10 @@
         <v>221</v>
       </c>
       <c r="D24" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E24" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F24" t="s">
         <v>160</v>
@@ -8108,16 +8117,16 @@
         <v>165</v>
       </c>
       <c r="I24" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J24" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K24" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="L24" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M24" t="s">
         <v>163</v>
@@ -8193,13 +8202,13 @@
         <v>255</v>
       </c>
       <c r="D26" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E26" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F26" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="G26" t="s">
         <v>256</v>
@@ -8211,13 +8220,13 @@
         <v>80</v>
       </c>
       <c r="J26" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K26" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="L26" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M26" t="s">
         <v>163</v>
@@ -8243,13 +8252,13 @@
         <v>160</v>
       </c>
       <c r="D27" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E27" t="s">
         <v>160</v>
       </c>
       <c r="F27" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="G27" t="s">
         <v>339</v>
@@ -8267,7 +8276,7 @@
         <v>80</v>
       </c>
       <c r="L27" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M27" t="s">
         <v>163</v>
@@ -8293,10 +8302,10 @@
         <v>179</v>
       </c>
       <c r="D28" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E28" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F28" t="s">
         <v>160</v>
@@ -8308,16 +8317,16 @@
         <v>182</v>
       </c>
       <c r="I28" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J28" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K28" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="L28" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M28" t="s">
         <v>163</v>
@@ -8393,10 +8402,10 @@
         <v>221</v>
       </c>
       <c r="D30" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E30" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F30" t="s">
         <v>160</v>
@@ -8408,16 +8417,16 @@
         <v>165</v>
       </c>
       <c r="I30" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J30" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K30" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="L30" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M30" t="s">
         <v>163</v>
@@ -8552,7 +8561,7 @@
         <v>80</v>
       </c>
       <c r="E33" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F33" t="s">
         <v>80</v>
@@ -8605,10 +8614,10 @@
         <v>160</v>
       </c>
       <c r="D34" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E34" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F34" t="s">
         <v>160</v>
@@ -8623,7 +8632,7 @@
         <v>80</v>
       </c>
       <c r="J34" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K34" t="s">
         <v>80</v>
@@ -8735,7 +8744,7 @@
         <v>80</v>
       </c>
       <c r="J36" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K36" t="s">
         <v>80</v>
@@ -8773,10 +8782,10 @@
         <v>160</v>
       </c>
       <c r="D37" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E37" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F37" t="s">
         <v>160</v>
@@ -8788,16 +8797,16 @@
         <v>182</v>
       </c>
       <c r="I37" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J37" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K37" t="s">
         <v>80</v>
       </c>
       <c r="L37" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M37" t="s">
         <v>163</v>
@@ -8847,7 +8856,7 @@
         <v>160</v>
       </c>
       <c r="J38" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K38" t="s">
         <v>160</v>
@@ -8885,10 +8894,10 @@
         <v>160</v>
       </c>
       <c r="D39" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E39" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F39" t="s">
         <v>160</v>
@@ -8903,13 +8912,13 @@
         <v>80</v>
       </c>
       <c r="J39" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K39" t="s">
         <v>80</v>
       </c>
       <c r="L39" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M39" t="s">
         <v>163</v>
@@ -8997,10 +9006,10 @@
         <v>160</v>
       </c>
       <c r="D41" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E41" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F41" t="s">
         <v>160</v>
@@ -9021,7 +9030,7 @@
         <v>80</v>
       </c>
       <c r="L41" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M41" t="s">
         <v>163</v>
@@ -9221,10 +9230,10 @@
         <v>160</v>
       </c>
       <c r="D45" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E45" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F45" t="s">
         <v>160</v>
@@ -9239,13 +9248,13 @@
         <v>80</v>
       </c>
       <c r="J45" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K45" t="s">
         <v>80</v>
       </c>
       <c r="L45" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M45" t="s">
         <v>163</v>
@@ -9280,7 +9289,7 @@
         <v>80</v>
       </c>
       <c r="E46" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F46" t="s">
         <v>160</v>
@@ -9295,13 +9304,13 @@
         <v>80</v>
       </c>
       <c r="J46" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K46" t="s">
         <v>80</v>
       </c>
       <c r="L46" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M46" t="s">
         <v>163</v>
@@ -9316,7 +9325,7 @@
         <v>160</v>
       </c>
       <c r="Q46" t="s">
-        <v>299</v>
+        <v>364</v>
       </c>
       <c r="R46" t="s">
         <v>160</v>
@@ -9333,10 +9342,10 @@
         <v>221</v>
       </c>
       <c r="D47" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E47" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F47" t="s">
         <v>160</v>
@@ -9348,22 +9357,22 @@
         <v>165</v>
       </c>
       <c r="I47" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J47" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K47" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="L47" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M47" t="s">
         <v>163</v>
       </c>
       <c r="N47" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="O47" t="s">
         <v>160</v>
@@ -9392,7 +9401,7 @@
         <v>80</v>
       </c>
       <c r="E48" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F48" t="s">
         <v>80</v>
@@ -9413,7 +9422,7 @@
         <v>80</v>
       </c>
       <c r="L48" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M48" t="s">
         <v>163</v>
@@ -9436,25 +9445,25 @@
     </row>
     <row r="49" spans="1:18">
       <c r="A49" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B49" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C49" t="s">
         <v>160</v>
       </c>
       <c r="D49" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E49" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F49" t="s">
         <v>160</v>
       </c>
       <c r="G49" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="H49" t="s">
         <v>73</v>
@@ -9463,22 +9472,22 @@
         <v>80</v>
       </c>
       <c r="J49" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="K49" t="s">
         <v>80</v>
       </c>
       <c r="L49" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="M49" t="s">
         <v>163</v>
       </c>
       <c r="N49" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="O49" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="P49" t="s">
         <v>160</v>
@@ -9531,7 +9540,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="B1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C1" t="s">
         <v>143</v>
@@ -9542,7 +9551,7 @@
         <v>199</v>
       </c>
       <c r="B2" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -9582,7 +9591,7 @@
         <v>214</v>
       </c>
       <c r="B7" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -9590,10 +9599,10 @@
         <v>334</v>
       </c>
       <c r="B8" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C8" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -9601,7 +9610,7 @@
         <v>224</v>
       </c>
       <c r="B9" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C9" t="s">
         <v>160</v>
@@ -9612,7 +9621,7 @@
         <v>282</v>
       </c>
       <c r="B10" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C10" t="s">
         <v>160</v>
@@ -9623,10 +9632,10 @@
         <v>190</v>
       </c>
       <c r="B11" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C11" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -9634,7 +9643,7 @@
         <v>170</v>
       </c>
       <c r="B12" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C12" t="s">
         <v>160</v>
@@ -9645,10 +9654,10 @@
         <v>322</v>
       </c>
       <c r="B13" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C13" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -9656,10 +9665,10 @@
         <v>330</v>
       </c>
       <c r="B14" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C14" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -9667,10 +9676,10 @@
         <v>244</v>
       </c>
       <c r="B15" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C15" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -9678,7 +9687,7 @@
         <v>167</v>
       </c>
       <c r="B16" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C16" t="s">
         <v>160</v>
@@ -9689,7 +9698,7 @@
         <v>253</v>
       </c>
       <c r="B17" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C17" t="s">
         <v>160</v>
@@ -9733,10 +9742,10 @@
         <v>345</v>
       </c>
       <c r="B21" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C21" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -9755,10 +9764,10 @@
         <v>359</v>
       </c>
       <c r="B23" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C23" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -9777,10 +9786,10 @@
         <v>319</v>
       </c>
       <c r="B25" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C25" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -9788,7 +9797,7 @@
         <v>287</v>
       </c>
       <c r="B26" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C26" t="s">
         <v>160</v>
@@ -9810,7 +9819,7 @@
         <v>297</v>
       </c>
       <c r="B28" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C28" t="s">
         <v>160</v>
@@ -9821,7 +9830,7 @@
         <v>300</v>
       </c>
       <c r="B29" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C29" t="s">
         <v>160</v>
@@ -9829,10 +9838,10 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B30" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C30" t="s">
         <v>160</v>
@@ -9879,13 +9888,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C1" t="s">
         <v>143</v>
       </c>
       <c r="D1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -9893,7 +9902,7 @@
         <v>199</v>
       </c>
       <c r="B2" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -9901,7 +9910,7 @@
         <v>229</v>
       </c>
       <c r="B3" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -9909,7 +9918,7 @@
         <v>310</v>
       </c>
       <c r="B4" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -9917,7 +9926,7 @@
         <v>203</v>
       </c>
       <c r="B5" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -9925,15 +9934,15 @@
         <v>209</v>
       </c>
       <c r="B6" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B7" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -9941,10 +9950,10 @@
         <v>334</v>
       </c>
       <c r="B8" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C8" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -9952,10 +9961,10 @@
         <v>190</v>
       </c>
       <c r="B9" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="C9" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -9963,7 +9972,7 @@
         <v>170</v>
       </c>
       <c r="B10" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="C10" t="s">
         <v>160</v>
@@ -9974,7 +9983,7 @@
         <v>322</v>
       </c>
       <c r="B11" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="C11" t="s">
         <v>160</v>
@@ -9985,10 +9994,10 @@
         <v>330</v>
       </c>
       <c r="B12" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="C12" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -9996,7 +10005,7 @@
         <v>167</v>
       </c>
       <c r="B13" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="C13" t="s">
         <v>160</v>
@@ -10007,7 +10016,7 @@
         <v>253</v>
       </c>
       <c r="B14" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C14" t="s">
         <v>160</v>
@@ -10018,7 +10027,7 @@
         <v>337</v>
       </c>
       <c r="B15" t="s">
-        <v>391</v>
+        <v>401</v>
       </c>
       <c r="C15" t="s">
         <v>160</v>
@@ -10029,7 +10038,7 @@
         <v>264</v>
       </c>
       <c r="B16" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="C16" t="s">
         <v>160</v>
@@ -10040,7 +10049,7 @@
         <v>345</v>
       </c>
       <c r="B17" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="C17" t="s">
         <v>160</v>
@@ -10051,7 +10060,7 @@
         <v>351</v>
       </c>
       <c r="B18" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="C18" t="s">
         <v>160</v>
@@ -10062,7 +10071,7 @@
         <v>359</v>
       </c>
       <c r="B19" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="C19" t="s">
         <v>160</v>
@@ -10073,7 +10082,7 @@
         <v>277</v>
       </c>
       <c r="B20" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="C20" t="s">
         <v>160</v>
@@ -10087,10 +10096,10 @@
         <v>160</v>
       </c>
       <c r="C21" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D21" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -10098,7 +10107,7 @@
         <v>304</v>
       </c>
       <c r="B22" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="C22" t="s">
         <v>160</v>
@@ -10112,7 +10121,7 @@
         <v>294</v>
       </c>
       <c r="B23" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="C23" t="s">
         <v>160</v>
@@ -10126,7 +10135,7 @@
         <v>297</v>
       </c>
       <c r="B24" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="C24" t="s">
         <v>160</v>
@@ -10140,7 +10149,7 @@
         <v>300</v>
       </c>
       <c r="B25" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C25" t="s">
         <v>160</v>
@@ -10151,10 +10160,10 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B26" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C26" t="s">
         <v>160</v>

</xml_diff>